<commit_message>
Fanta teams added clickable link
</commit_message>
<xml_diff>
--- a/Excel/Milano/FantaSPL_Classifica.xlsx
+++ b/Excel/Milano/FantaSPL_Classifica.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Player Name</t>
+          <t>Rank</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -449,71 +449,49 @@
           <t>Total Points Scored</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Rank</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Matteo Ciccaldo</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SPL:Solo Per Letette (ciccu)</t>
+          <t>Limonta United</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>72</v>
-      </c>
-      <c r="D2" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Andrea Limonta</t>
-        </is>
-      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Limonta United</t>
+          <t>Football Meta Academy</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>67</v>
       </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cormac McAinsh</t>
-        </is>
+      <c r="A4" t="n">
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Football Meta Academy</t>
+          <t>SPL:Solo Per Letette (ciccu)</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>67</v>
       </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ilona Urban</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -523,15 +501,10 @@
       <c r="C5" t="n">
         <v>65</v>
       </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Omar Raafat</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -541,15 +514,10 @@
       <c r="C6" t="n">
         <v>63</v>
       </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Maurizio Rea</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -559,15 +527,10 @@
       <c r="C7" t="n">
         <v>61</v>
       </c>
-      <c r="D7" t="n">
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sergio Cavalieri</t>
-        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -577,15 +540,10 @@
       <c r="C8" t="n">
         <v>61</v>
       </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Mazzucchello Lorenzi</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -595,15 +553,10 @@
       <c r="C9" t="n">
         <v>59</v>
       </c>
-      <c r="D9" t="n">
-        <v>8</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Daniele Miccoli</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -613,15 +566,10 @@
       <c r="C10" t="n">
         <v>58</v>
       </c>
-      <c r="D10" t="n">
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ludovico Righi</t>
-        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -631,15 +579,10 @@
       <c r="C11" t="n">
         <v>58</v>
       </c>
-      <c r="D11" t="n">
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>9</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Roberto Janni</t>
-        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -649,51 +592,36 @@
       <c r="C12" t="n">
         <v>58</v>
       </c>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ilaria Pascutti</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Mazzu è ok</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>Cesarino’s</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>57</v>
-      </c>
-      <c r="D13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Marzio lorenzelli</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Mazzu è ok</t>
-        </is>
-      </c>
       <c r="C14" t="n">
-        <v>54</v>
-      </c>
-      <c r="D14" t="n">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Lorenzo Mazzucchelli</t>
-        </is>
+      <c r="A15" t="n">
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -703,15 +631,10 @@
       <c r="C15" t="n">
         <v>51</v>
       </c>
-      <c r="D15" t="n">
-        <v>14</v>
-      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Damiano Barbanera</t>
-        </is>
+      <c r="A16" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -721,15 +644,10 @@
       <c r="C16" t="n">
         <v>50</v>
       </c>
-      <c r="D16" t="n">
-        <v>15</v>
-      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Federico Lelli</t>
-        </is>
+      <c r="A17" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -739,15 +657,10 @@
       <c r="C17" t="n">
         <v>47</v>
       </c>
-      <c r="D17" t="n">
-        <v>16</v>
-      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Cristian Diaz Lopez</t>
-        </is>
+      <c r="A18" t="n">
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -757,15 +670,10 @@
       <c r="C18" t="n">
         <v>45</v>
       </c>
-      <c r="D18" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Federico Paolucci</t>
-        </is>
+      <c r="A19" t="n">
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -775,69 +683,49 @@
       <c r="C19" t="n">
         <v>42</v>
       </c>
-      <c r="D19" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Manuel Maimone</t>
-        </is>
+      <c r="A20" t="n">
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Fury Bonds</t>
+          <t>Affori Grizzlies</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>40</v>
-      </c>
-      <c r="D20" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Giovanni Aiello</t>
-        </is>
-      </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Affori Grizzlies</t>
+          <t>I nemici di mazzu</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>39</v>
       </c>
-      <c r="D21" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Arturo Guglielmi</t>
-        </is>
+      <c r="A22" t="n">
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>I nemici di mazzu</t>
+          <t>Fury Bonds</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>39</v>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Fabrizio Limonta</t>
-        </is>
+      <c r="A23" t="n">
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -847,15 +735,10 @@
       <c r="C23" t="n">
         <v>33</v>
       </c>
-      <c r="D23" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Cameron McAinsh</t>
-        </is>
+      <c r="A24" t="n">
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -864,9 +747,6 @@
       </c>
       <c r="C24" t="n">
         <v>9</v>
-      </c>
-      <c r="D24" t="n">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Season 2 results eliminated
</commit_message>
<xml_diff>
--- a/Excel/Milano/FantaSPL_Classifica.xlsx
+++ b/Excel/Milano/FantaSPL_Classifica.xlsx
@@ -456,297 +456,297 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Omanta</t>
+          <t>Limonta United</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPL Solo Per Letette (ciccu)</t>
+          <t>Caledonians</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I nemici di mazzu</t>
+          <t>Rapid Viennetta</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Caledonians</t>
+          <t>Omanta</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LA PALLA NON ERA USCITA</t>
+          <t>Non è la seconda squadra di Mazzu, è la prima</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Multiple Cancers</t>
+          <t>T'eamCulo</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rapid Viennetta</t>
+          <t>SPL Solo Per Letette (ciccu)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Football Meta Academy</t>
+          <t>Mazzu è ok</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Affori Grizzlies</t>
+          <t>Fury Bonds</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mazzu doveva Vincere</t>
+          <t>LA PALLA NON ERA USCITA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Non è la seconda squadra di Mazzu, è la prima</t>
+          <t>Mazzu doveva Vincere</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Beverly INPS</t>
+          <t>Cesarino’s</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Latin Supremacy</t>
+          <t>I nemici di mazzu</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mazzu è ok</t>
+          <t>Affori Grizzlies</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Aldo Ritmo</t>
+          <t>Beverly INPS</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BARBA FC</t>
+          <t>Multiple Cancers</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>T'eamCulo</t>
+          <t>Fel Lazio</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CHIAVO VERONA</t>
+          <t>Aldo Ritmo</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Limonta United</t>
+          <t>BARBA FC</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cesarino’s</t>
+          <t>Latin Supremacy</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fel Lazio</t>
+          <t>Football Meta Academy</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fury Bonds</t>
+          <t>Artificially Degenerated</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Artificially Degenerated</t>
+          <t>CHIAVO VERONA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Game results - official
</commit_message>
<xml_diff>
--- a/Excel/Milano/FantaSPL_Classifica.xlsx
+++ b/Excel/Milano/FantaSPL_Classifica.xlsx
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
@@ -495,11 +495,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CHIAVO VERONA</t>
+          <t>Omanta</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -508,11 +508,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Beverly INPS</t>
+          <t>CHIAVO VERONA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -521,24 +521,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fel Lazio</t>
+          <t>Beverly INPS</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Omanta</t>
+          <t>Rahal Madrid</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -547,46 +547,46 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rahal Madrid</t>
+          <t>T'eamCulo</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mazzu è ok</t>
+          <t>AC Tua</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Non è la seconda squadra di Mazzu, è la prima</t>
+          <t>Fel Lazio</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Artificially Degenerated</t>
+          <t>Football Meta Academy</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -595,80 +595,80 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>T'eamCulo</t>
+          <t>Non è la seconda squadra di Mazzu, è la prima</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AC Tua</t>
+          <t>SPL Solo Per Letette</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Limonta United</t>
+          <t>Mazzu è ok</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sesso Paperoga Lamborghini</t>
+          <t>Rapid Viennetta</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Football Meta Academy</t>
+          <t>Calabria Saudita</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SPL Solo Per Letette</t>
+          <t>Limonta United</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
@@ -677,24 +677,24 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Rapid Viennetta</t>
+          <t>Artificially Degenerated</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Calabria Saudita</t>
+          <t>Sesso Paperoga Lamborghini</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21">
@@ -703,11 +703,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Slayer FC</t>
+          <t>Affori Grizzlies</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22">
@@ -716,11 +716,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Affori Grizzlies</t>
+          <t>Si è girato Mazzoud</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
@@ -729,16 +729,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Si è girato Mazzoud</t>
+          <t>Slayer FC</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -755,11 +755,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BaffoImpregnato</t>
+          <t>Aldo Ritmo</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26">
@@ -768,11 +768,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>NonCiCapiscoNaMazza</t>
+          <t>BaffoImpregnato</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27">
@@ -781,11 +781,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Aldo Ritmo</t>
+          <t>NonCiCapiscoNaMazza</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
MVP and SPL added
</commit_message>
<xml_diff>
--- a/Excel/Milano/FantaSPL_Classifica.xlsx
+++ b/Excel/Milano/FantaSPL_Classifica.xlsx
@@ -52,12 +52,12 @@
     <t>Mazzu è ok</t>
   </si>
   <si>
+    <t>Olesto</t>
+  </si>
+  <si>
     <t>Affori Grizzlies</t>
   </si>
   <si>
-    <t>Olesto</t>
-  </si>
-  <si>
     <t>Frozzynone</t>
   </si>
   <si>
@@ -91,28 +91,28 @@
     <t>BaffoImpregnato</t>
   </si>
   <si>
+    <t>Slayer FC</t>
+  </si>
+  <si>
     <t>Beverly INPS</t>
   </si>
   <si>
-    <t>Slayer FC</t>
+    <t>T'eamCulo</t>
   </si>
   <si>
     <t>Multiple Cancers</t>
   </si>
   <si>
-    <t>T'eamCulo</t>
-  </si>
-  <si>
     <t>AC Tua</t>
   </si>
   <si>
     <t>AS TRONZI</t>
   </si>
   <si>
+    <t>Fel Lazio</t>
+  </si>
+  <si>
     <t>Damiano Zingaro</t>
-  </si>
-  <si>
-    <t>Fel Lazio</t>
   </si>
   <si>
     <t>Sesso Paperoga Lamborghini</t>
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -536,12 +536,12 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -569,7 +569,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -591,7 +591,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -607,13 +607,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -624,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -635,7 +635,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -657,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -668,7 +668,7 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -679,7 +679,7 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>441</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -690,7 +690,7 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -756,7 +756,7 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -767,12 +767,12 @@
         <v>25</v>
       </c>
       <c r="C24">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -789,12 +789,12 @@
         <v>27</v>
       </c>
       <c r="C26">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -833,7 +833,7 @@
         <v>31</v>
       </c>
       <c r="C30">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -844,7 +844,7 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -855,7 +855,7 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -877,7 +877,7 @@
         <v>35</v>
       </c>
       <c r="C34">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -910,7 +910,7 @@
         <v>38</v>
       </c>
       <c r="C37">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:3">

</xml_diff>